<commit_message>
updated timing output excel
</commit_message>
<xml_diff>
--- a/Outputs/timings_output.xlsx
+++ b/Outputs/timings_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMARTlabUSER\OneDrive - George Mason University - O365 Production\Documents 1\Git Hub\VSCODE\Tug_Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patk1\OneDrive\Desktop\Git Hub\Tug_Test\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA167045-46E5-4CC7-8CCE-67DD4E8BAFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF71F07-0393-49FB-9EB1-256DBFA7036C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="77">
   <si>
     <t>Trial</t>
   </si>
@@ -136,6 +136,15 @@
     <t>20240227-114755EST_TUG_Trial.csv</t>
   </si>
   <si>
+    <t>20240311-161016EDT_TUG_Trial.csv</t>
+  </si>
+  <si>
+    <t>20240311-161051EDT_TUG_Trial.csv</t>
+  </si>
+  <si>
+    <t>20240311-161130EDT_TUG_Trial.csv</t>
+  </si>
+  <si>
     <t>20231109-150313EST_TUG_Trial.csv</t>
   </si>
   <si>
@@ -224,6 +233,15 @@
   </si>
   <si>
     <t>20240227-113816EST_TUG_Trial.csv</t>
+  </si>
+  <si>
+    <t>20240311-160513EDT_TUG_Trial.csv</t>
+  </si>
+  <si>
+    <t>20240311-160628EDT_TUG_Trial.csv</t>
+  </si>
+  <si>
+    <t>20240311-160814EDT_TUG_Trial.csv</t>
   </si>
   <si>
     <t>[]</t>
@@ -314,9 +332,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,9 +372,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,26 +407,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,26 +442,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,25 +618,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="33.109375" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -698,13 +681,13 @@
         <v>0.24496644295302011</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -724,13 +707,13 @@
         <v>0.223760092272203</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -750,13 +733,13 @@
         <v>0.1933404940923738</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -776,13 +759,13 @@
         <v>0.27007299270072987</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -802,13 +785,13 @@
         <v>0.17027281279397929</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -828,13 +811,13 @@
         <v>0.248015873015873</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -854,13 +837,13 @@
         <v>0.20796890184645289</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -880,13 +863,13 @@
         <v>0.195357833655706</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -906,13 +889,13 @@
         <v>0.21041879468845759</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -932,13 +915,13 @@
         <v>0.21992110453648911</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -958,13 +941,13 @@
         <v>0.25899280575539568</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -984,13 +967,13 @@
         <v>0.25</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1010,13 +993,13 @@
         <v>0.19554848966613669</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1036,13 +1019,13 @@
         <v>0.16279069767441859</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1062,13 +1045,13 @@
         <v>0.18592964824120611</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1088,13 +1071,13 @@
         <v>0.20806599450045829</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1114,13 +1097,13 @@
         <v>0.2061005770816158</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1140,13 +1123,13 @@
         <v>0.18110236220472439</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1166,13 +1149,13 @@
         <v>0.20920201294033069</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1192,13 +1175,13 @@
         <v>0.20594965675057211</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1218,13 +1201,13 @@
         <v>0.20610687022900759</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1244,13 +1227,13 @@
         <v>0.22171945701357471</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1270,13 +1253,13 @@
         <v>0.2463054187192118</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1296,13 +1279,13 @@
         <v>0.29573170731707321</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1322,13 +1305,13 @@
         <v>0.24313725490196081</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1348,13 +1331,13 @@
         <v>0.2406902815622162</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1374,13 +1357,13 @@
         <v>0.2448614834673816</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1400,13 +1383,13 @@
         <v>0.21281840591618731</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1426,13 +1409,13 @@
         <v>0.11497005988023951</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1452,790 +1435,946 @@
         <v>7.8646092583374821E-2</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
       <c r="B32">
-        <v>9.1300000000000008</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C32">
-        <v>0.84</v>
+        <v>0.8</v>
       </c>
       <c r="D32">
-        <v>2.44</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="E32">
-        <v>9.2004381161007662E-2</v>
+        <v>9.195402298850576E-2</v>
       </c>
       <c r="F32">
-        <v>0.26725082146768891</v>
+        <v>0.25517241379310351</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33">
-        <v>8.52</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="C33">
-        <v>0.86</v>
+        <v>0.79</v>
       </c>
       <c r="D33">
-        <v>1.98</v>
+        <v>1.73</v>
       </c>
       <c r="E33">
-        <v>0.10093896713615021</v>
+        <v>8.7292817679558002E-2</v>
       </c>
       <c r="F33">
-        <v>0.23239436619718309</v>
+        <v>0.19116022099447511</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
       <c r="B34">
-        <v>9.23</v>
+        <v>8.83</v>
       </c>
       <c r="C34">
-        <v>0.79</v>
+        <v>0.84</v>
       </c>
       <c r="D34">
-        <v>2.4900000000000002</v>
+        <v>2.25</v>
       </c>
       <c r="E34">
-        <v>8.5590465872156019E-2</v>
+        <v>9.5130237825594557E-2</v>
       </c>
       <c r="F34">
-        <v>0.26977248104008672</v>
+        <v>0.25481313703284258</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
       <c r="B35">
-        <v>10.3</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="C35">
-        <v>1.23</v>
+        <v>0.84</v>
       </c>
       <c r="D35">
-        <v>1.96</v>
+        <v>2.44</v>
       </c>
       <c r="E35">
-        <v>0.1194174757281553</v>
+        <v>9.2004381161007662E-2</v>
       </c>
       <c r="F35">
-        <v>0.19029126213592229</v>
+        <v>0.26725082146768891</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
       <c r="B36">
-        <v>9.61</v>
+        <v>8.52</v>
       </c>
       <c r="C36">
-        <v>1.1200000000000001</v>
+        <v>0.86</v>
       </c>
       <c r="D36">
-        <v>2.37</v>
+        <v>1.98</v>
       </c>
       <c r="E36">
-        <v>0.1165452653485952</v>
+        <v>0.10093896713615021</v>
       </c>
       <c r="F36">
-        <v>0.2466181061394381</v>
+        <v>0.23239436619718309</v>
       </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
       <c r="B37">
-        <v>8.52</v>
+        <v>9.23</v>
       </c>
       <c r="C37">
-        <v>1.19</v>
+        <v>0.79</v>
       </c>
       <c r="D37">
-        <v>1.91</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="E37">
-        <v>0.13967136150234741</v>
+        <v>8.5590465872156019E-2</v>
       </c>
       <c r="F37">
-        <v>0.2241784037558685</v>
+        <v>0.26977248104008672</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38">
-        <v>10.77</v>
+        <v>10.3</v>
       </c>
       <c r="C38">
-        <v>1.1100000000000001</v>
+        <v>1.23</v>
       </c>
       <c r="D38">
-        <v>2.59</v>
+        <v>1.96</v>
       </c>
       <c r="E38">
-        <v>0.1030640668523677</v>
+        <v>0.1194174757281553</v>
       </c>
       <c r="F38">
-        <v>0.24048282265552459</v>
+        <v>0.19029126213592229</v>
       </c>
       <c r="G38" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39">
-        <v>9.6300000000000008</v>
+        <v>9.61</v>
       </c>
       <c r="C39">
-        <v>1.07</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D39">
-        <v>1.87</v>
+        <v>2.37</v>
       </c>
       <c r="E39">
-        <v>0.1111111111111111</v>
+        <v>0.1165452653485952</v>
       </c>
       <c r="F39">
-        <v>0.19418483904465211</v>
+        <v>0.2466181061394381</v>
       </c>
       <c r="G39" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
       <c r="B40">
-        <v>9.24</v>
+        <v>8.52</v>
       </c>
       <c r="C40">
-        <v>1.23</v>
+        <v>1.19</v>
       </c>
       <c r="D40">
-        <v>1.99</v>
+        <v>1.91</v>
       </c>
       <c r="E40">
-        <v>0.13311688311688311</v>
+        <v>0.13967136150234741</v>
       </c>
       <c r="F40">
-        <v>0.2153679653679654</v>
+        <v>0.2241784037558685</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
       <c r="B41">
-        <v>9.61</v>
+        <v>10.77</v>
       </c>
       <c r="C41">
-        <v>0.67</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D41">
-        <v>2.02</v>
+        <v>2.59</v>
       </c>
       <c r="E41">
-        <v>6.9719042663891784E-2</v>
+        <v>0.1030640668523677</v>
       </c>
       <c r="F41">
-        <v>0.21019771071800211</v>
+        <v>0.24048282265552459</v>
       </c>
       <c r="G41" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
       <c r="B42">
-        <v>9.19</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="C42">
-        <v>0.83</v>
+        <v>1.07</v>
       </c>
       <c r="D42">
-        <v>2.42</v>
+        <v>1.87</v>
       </c>
       <c r="E42">
-        <v>9.0315560391730138E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F42">
-        <v>0.26332970620239388</v>
+        <v>0.19418483904465211</v>
       </c>
       <c r="G42" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43">
-        <v>9.11</v>
+        <v>9.24</v>
       </c>
       <c r="C43">
-        <v>0.75</v>
+        <v>1.23</v>
       </c>
       <c r="D43">
-        <v>2.4700000000000002</v>
+        <v>1.99</v>
       </c>
       <c r="E43">
-        <v>8.232711306256861E-2</v>
+        <v>0.13311688311688311</v>
       </c>
       <c r="F43">
-        <v>0.27113062568605928</v>
+        <v>0.2153679653679654</v>
       </c>
       <c r="G43" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="B44">
-        <v>11.23</v>
+        <v>9.61</v>
       </c>
       <c r="C44">
-        <v>1.25</v>
+        <v>0.67</v>
       </c>
       <c r="D44">
-        <v>2.39</v>
+        <v>2.02</v>
       </c>
       <c r="E44">
-        <v>0.1113089937666963</v>
+        <v>6.9719042663891784E-2</v>
       </c>
       <c r="F44">
-        <v>0.21282279608192339</v>
+        <v>0.21019771071800211</v>
       </c>
       <c r="G44" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
       <c r="B45">
-        <v>11.01</v>
+        <v>9.19</v>
       </c>
       <c r="C45">
-        <v>1.38</v>
+        <v>0.83</v>
       </c>
       <c r="D45">
-        <v>1.87</v>
+        <v>2.42</v>
       </c>
       <c r="E45">
-        <v>0.12534059945504089</v>
+        <v>9.0315560391730138E-2</v>
       </c>
       <c r="F45">
-        <v>0.16984559491371479</v>
+        <v>0.26332970620239388</v>
       </c>
       <c r="G45" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
       <c r="B46">
-        <v>10.78</v>
+        <v>9.11</v>
       </c>
       <c r="C46">
-        <v>1.38</v>
+        <v>0.75</v>
       </c>
       <c r="D46">
-        <v>2.1</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="E46">
-        <v>0.1280148423005566</v>
+        <v>8.232711306256861E-2</v>
       </c>
       <c r="F46">
-        <v>0.19480519480519479</v>
+        <v>0.27113062568605928</v>
       </c>
       <c r="G46" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
       <c r="B47">
-        <v>9.84</v>
+        <v>11.23</v>
       </c>
       <c r="C47">
-        <v>0.99</v>
+        <v>1.25</v>
       </c>
       <c r="D47">
-        <v>2.0699999999999998</v>
+        <v>2.39</v>
       </c>
       <c r="E47">
-        <v>0.100609756097561</v>
+        <v>0.1113089937666963</v>
       </c>
       <c r="F47">
-        <v>0.21036585365853661</v>
+        <v>0.21282279608192339</v>
       </c>
       <c r="G47" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
       <c r="B48">
-        <v>8.9700000000000006</v>
+        <v>11.01</v>
       </c>
       <c r="C48">
-        <v>0.93</v>
+        <v>1.38</v>
       </c>
       <c r="D48">
-        <v>2.19</v>
+        <v>1.87</v>
       </c>
       <c r="E48">
-        <v>0.1036789297658863</v>
+        <v>0.12534059945504089</v>
       </c>
       <c r="F48">
-        <v>0.2441471571906354</v>
+        <v>0.16984559491371479</v>
       </c>
       <c r="G48" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
       <c r="B49">
-        <v>8.59</v>
+        <v>10.78</v>
       </c>
       <c r="C49">
-        <v>0.87</v>
+        <v>1.38</v>
       </c>
       <c r="D49">
-        <v>2.29</v>
+        <v>2.1</v>
       </c>
       <c r="E49">
-        <v>0.1012805587892899</v>
+        <v>0.1280148423005566</v>
       </c>
       <c r="F49">
-        <v>0.26658905704307329</v>
+        <v>0.19480519480519479</v>
       </c>
       <c r="G49" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
       <c r="B50">
-        <v>10.68</v>
+        <v>9.84</v>
       </c>
       <c r="C50">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="D50">
-        <v>2.04</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E50">
-        <v>8.98876404494382E-2</v>
+        <v>0.100609756097561</v>
       </c>
       <c r="F50">
-        <v>0.1910112359550562</v>
+        <v>0.21036585365853661</v>
       </c>
       <c r="G50" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H50" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
       <c r="B51">
-        <v>10.51</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="C51">
-        <v>1.02</v>
+        <v>0.93</v>
       </c>
       <c r="D51">
-        <v>2.09</v>
+        <v>2.19</v>
       </c>
       <c r="E51">
-        <v>9.7050428163653668E-2</v>
+        <v>0.1036789297658863</v>
       </c>
       <c r="F51">
-        <v>0.19885823025689819</v>
+        <v>0.2441471571906354</v>
       </c>
       <c r="G51" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
       <c r="B52">
-        <v>10.53</v>
+        <v>8.59</v>
       </c>
       <c r="C52">
-        <v>0.99</v>
+        <v>0.87</v>
       </c>
       <c r="D52">
-        <v>2.27</v>
+        <v>2.29</v>
       </c>
       <c r="E52">
-        <v>9.4017094017094016E-2</v>
+        <v>0.1012805587892899</v>
       </c>
       <c r="F52">
-        <v>0.21557454890788219</v>
+        <v>0.26658905704307329</v>
       </c>
       <c r="G52" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
       <c r="B53">
-        <v>6.22</v>
+        <v>10.68</v>
       </c>
       <c r="C53">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="D53">
-        <v>1.28</v>
+        <v>2.04</v>
       </c>
       <c r="E53">
-        <v>0.15273311897106109</v>
+        <v>8.98876404494382E-2</v>
       </c>
       <c r="F53">
-        <v>0.20578778135048231</v>
+        <v>0.1910112359550562</v>
       </c>
       <c r="G53" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
       <c r="B54">
-        <v>6.14</v>
+        <v>10.51</v>
       </c>
       <c r="C54">
-        <v>0.88</v>
+        <v>1.02</v>
       </c>
       <c r="D54">
-        <v>1.19</v>
+        <v>2.09</v>
       </c>
       <c r="E54">
-        <v>0.14332247557003261</v>
+        <v>9.7050428163653668E-2</v>
       </c>
       <c r="F54">
-        <v>0.19381107491856681</v>
+        <v>0.19885823025689819</v>
       </c>
       <c r="G54" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
       <c r="B55">
-        <v>6.2</v>
+        <v>10.53</v>
       </c>
       <c r="C55">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
       <c r="D55">
-        <v>1.48</v>
+        <v>2.27</v>
       </c>
       <c r="E55">
-        <v>0.15</v>
+        <v>9.4017094017094016E-2</v>
       </c>
       <c r="F55">
-        <v>0.23870967741935481</v>
+        <v>0.21557454890788219</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
       <c r="B56">
-        <v>7.83</v>
+        <v>6.22</v>
       </c>
       <c r="C56">
-        <v>1.06</v>
+        <v>0.95</v>
       </c>
       <c r="D56">
-        <v>1.71</v>
+        <v>1.28</v>
       </c>
       <c r="E56">
-        <v>0.13537675606641131</v>
+        <v>0.15273311897106109</v>
       </c>
       <c r="F56">
-        <v>0.2183908045977011</v>
+        <v>0.20578778135048231</v>
       </c>
       <c r="G56" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
       <c r="B57">
-        <v>7.49</v>
+        <v>6.14</v>
       </c>
       <c r="C57">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="D57">
-        <v>2.06</v>
+        <v>1.19</v>
       </c>
       <c r="E57">
-        <v>0.1201602136181575</v>
+        <v>0.14332247557003261</v>
       </c>
       <c r="F57">
-        <v>0.27503337783711618</v>
+        <v>0.19381107491856681</v>
       </c>
       <c r="G57" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
       <c r="B58">
-        <v>8.65</v>
+        <v>6.2</v>
       </c>
       <c r="C58">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="D58">
-        <v>2.2799999999999998</v>
+        <v>1.48</v>
       </c>
       <c r="E58">
-        <v>0.1052023121387283</v>
+        <v>0.15</v>
       </c>
       <c r="F58">
-        <v>0.26358381502890171</v>
+        <v>0.23870967741935481</v>
       </c>
       <c r="G58" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
       <c r="B59">
-        <v>11.12</v>
+        <v>7.83</v>
       </c>
       <c r="C59">
-        <v>1.03</v>
+        <v>1.06</v>
       </c>
       <c r="D59">
-        <v>1.98</v>
+        <v>1.71</v>
       </c>
       <c r="E59">
-        <v>9.2625899280575547E-2</v>
+        <v>0.13537675606641131</v>
       </c>
       <c r="F59">
-        <v>0.17805755395683451</v>
+        <v>0.2183908045977011</v>
       </c>
       <c r="G59" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
       <c r="B60">
-        <v>10.73</v>
+        <v>7.49</v>
       </c>
       <c r="C60">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="D60">
-        <v>2.0099999999999998</v>
+        <v>2.06</v>
       </c>
       <c r="E60">
-        <v>9.5060577819198508E-2</v>
+        <v>0.1201602136181575</v>
       </c>
       <c r="F60">
-        <v>0.18732525629077351</v>
+        <v>0.27503337783711618</v>
       </c>
       <c r="G60" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
       <c r="B61">
+        <v>8.65</v>
+      </c>
+      <c r="C61">
+        <v>0.91</v>
+      </c>
+      <c r="D61">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E61">
+        <v>0.1052023121387283</v>
+      </c>
+      <c r="F61">
+        <v>0.26358381502890171</v>
+      </c>
+      <c r="G61" t="s">
+        <v>74</v>
+      </c>
+      <c r="H61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62">
+        <v>11.12</v>
+      </c>
+      <c r="C62">
+        <v>1.03</v>
+      </c>
+      <c r="D62">
+        <v>1.98</v>
+      </c>
+      <c r="E62">
+        <v>9.2625899280575547E-2</v>
+      </c>
+      <c r="F62">
+        <v>0.17805755395683451</v>
+      </c>
+      <c r="G62" t="s">
+        <v>74</v>
+      </c>
+      <c r="H62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63">
+        <v>10.73</v>
+      </c>
+      <c r="C63">
+        <v>1.02</v>
+      </c>
+      <c r="D63">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E63">
+        <v>9.5060577819198508E-2</v>
+      </c>
+      <c r="F63">
+        <v>0.18732525629077351</v>
+      </c>
+      <c r="G63" t="s">
+        <v>74</v>
+      </c>
+      <c r="H63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64">
         <v>10.94</v>
       </c>
-      <c r="C61">
+      <c r="C64">
         <v>1.02</v>
       </c>
-      <c r="D61">
+      <c r="D64">
         <v>2.3199999999999998</v>
       </c>
-      <c r="E61">
+      <c r="E64">
         <v>9.3235831809872036E-2</v>
       </c>
-      <c r="F61">
+      <c r="F64">
         <v>0.21206581352833639</v>
       </c>
-      <c r="G61" t="s">
-        <v>68</v>
-      </c>
-      <c r="H61" t="s">
-        <v>70</v>
+      <c r="G64" t="s">
+        <v>74</v>
+      </c>
+      <c r="H64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65">
+        <v>8.44</v>
+      </c>
+      <c r="C65">
+        <v>0.81</v>
+      </c>
+      <c r="D65">
+        <v>2.16</v>
+      </c>
+      <c r="E65">
+        <v>9.597156398104266E-2</v>
+      </c>
+      <c r="F65">
+        <v>0.25592417061611378</v>
+      </c>
+      <c r="G65" t="s">
+        <v>74</v>
+      </c>
+      <c r="H65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66">
+        <v>8.39</v>
+      </c>
+      <c r="C66">
+        <v>0.8</v>
+      </c>
+      <c r="D66">
+        <v>2.25</v>
+      </c>
+      <c r="E66">
+        <v>9.5351609058402856E-2</v>
+      </c>
+      <c r="F66">
+        <v>0.268176400476758</v>
+      </c>
+      <c r="G66" t="s">
+        <v>74</v>
+      </c>
+      <c r="H66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67">
+        <v>7.74</v>
+      </c>
+      <c r="C67">
+        <v>0.59</v>
+      </c>
+      <c r="D67">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E67">
+        <v>7.622739018087854E-2</v>
+      </c>
+      <c r="F67">
+        <v>0.28165374677002591</v>
+      </c>
+      <c r="G67" t="s">
+        <v>74</v>
+      </c>
+      <c r="H67" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>